<commit_message>
v. 1.2 ST [addr], A instruction implemented, not tested yet
</commit_message>
<xml_diff>
--- a/1st gen - 4 bit cpu/Instruction Set.xlsx
+++ b/1st gen - 4 bit cpu/Instruction Set.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="754" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="754" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Multiply program code" sheetId="2" r:id="rId2"/>
-    <sheet name="Test program 1" sheetId="3" r:id="rId3"/>
-    <sheet name="Test program 2" sheetId="4" r:id="rId4"/>
-    <sheet name="Test program 3" sheetId="5" r:id="rId5"/>
-    <sheet name="Test program 4" sheetId="6" r:id="rId6"/>
-    <sheet name="Test program 5" sheetId="7" r:id="rId7"/>
-    <sheet name="Test program 6" sheetId="8" r:id="rId8"/>
-    <sheet name="Test program 7" sheetId="9" r:id="rId9"/>
+    <sheet name="Test program 1" sheetId="3" r:id="rId2"/>
+    <sheet name="Test program 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Test program 3" sheetId="5" r:id="rId4"/>
+    <sheet name="Test program 4" sheetId="6" r:id="rId5"/>
+    <sheet name="Test program 5" sheetId="7" r:id="rId6"/>
+    <sheet name="Test program 6" sheetId="8" r:id="rId7"/>
+    <sheet name="Test program 7" sheetId="9" r:id="rId8"/>
+    <sheet name="Multiply program code" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -1166,186 +1166,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
@@ -1545,11 +1365,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1692,7 +1512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -1838,7 +1658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -2037,7 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -2208,7 +2028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -2429,7 +2249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -2575,4 +2395,184 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented instruction ST [addr], A. All 10 instructions working. POC finished.
</commit_message>
<xml_diff>
--- a/1st gen - 4 bit cpu/Instruction Set.xlsx
+++ b/1st gen - 4 bit cpu/Instruction Set.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="754" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="754" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,15 @@
     <sheet name="Test program 5" sheetId="7" r:id="rId6"/>
     <sheet name="Test program 6" sheetId="8" r:id="rId7"/>
     <sheet name="Test program 7" sheetId="9" r:id="rId8"/>
-    <sheet name="Multiply program code" sheetId="2" r:id="rId9"/>
+    <sheet name="Test program 8" sheetId="10" r:id="rId9"/>
+    <sheet name="Multiply program code" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="171">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -520,6 +521,21 @@
   </si>
   <si>
     <t>Copies the value of memory address 8h to the register A</t>
+  </si>
+  <si>
+    <t>ST [1h], A</t>
+  </si>
+  <si>
+    <t>11011001</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>11110002</t>
+  </si>
+  <si>
+    <t>Copies the value of memory address 8h to the register A, and then to the memory position 9h (remembering it's started at 8h for Load/Store operations)</t>
   </si>
 </sst>
 </file>
@@ -883,7 +899,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,6 +1175,186 @@
   <ignoredErrors>
     <ignoredError sqref="B3" numberStoredAsText="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1369,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2254,7 +2450,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="J12" sqref="A1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,36 +2597,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>164</v>
       </c>
       <c r="G2" t="s">
         <v>22</v>
@@ -2444,13 +2646,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -2464,13 +2666,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>169</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -2483,15 +2685,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="G5" t="s">
         <v>25</v>
       </c>
@@ -2503,15 +2697,8 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="G6" t="s">
         <v>26</v>
       </c>
@@ -2523,15 +2710,8 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="G7" t="s">
         <v>27</v>
       </c>
@@ -2543,36 +2723,29 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>140</v>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>141</v>
+      <c r="E12" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>